<commit_message>
Daniel Cambios de main.py, introduccion prompts, ausencia medicion_prompts
</commit_message>
<xml_diff>
--- a/script_master_data_beltran/ficherosExcelOrigen/DED-NAUA_Plantilla_Adopcion IA.xlsx
+++ b/script_master_data_beltran/ficherosExcelOrigen/DED-NAUA_Plantilla_Adopcion IA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF5894B-F6F4-420D-8542-9082FF57B71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9267CFB5-8C02-4EC2-BDB9-67100C61D20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16125" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-16125" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdopcionIA" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="459">
   <si>
     <t>GISS-DED - Adopción IA: &lt;Proyecto XXX&gt;</t>
   </si>
@@ -1430,6 +1430,15 @@
   </si>
   <si>
     <t>Media Calidad</t>
+  </si>
+  <si>
+    <t>prompts</t>
+  </si>
+  <si>
+    <t>Analisis Desa APIs</t>
+  </si>
+  <si>
+    <t>Comprender Codigo Fuente</t>
   </si>
 </sst>
 </file>
@@ -21517,10 +21526,10 @@
   <dimension ref="A1:BS197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="AQ6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomRight" activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21534,10 +21543,11 @@
     <col min="42" max="42" width="94.453125" style="133" customWidth="1"/>
     <col min="43" max="43" width="29.1796875" style="1" customWidth="1"/>
     <col min="44" max="44" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="46" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J1" s="1">
         <f>SUM(J6:J155)</f>
         <v>14.849999999999989</v>
@@ -21571,19 +21581,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:45" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="81"/>
       <c r="B3" s="81" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:44" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
         <v>2</v>
@@ -21635,7 +21645,7 @@
       <c r="AO4" s="6"/>
       <c r="AP4" s="134"/>
     </row>
-    <row r="5" spans="1:44" ht="40" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:45" ht="40" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -21768,8 +21778,11 @@
       <c r="AR5" s="25" t="s">
         <v>21</v>
       </c>
+      <c r="AS5" t="s">
+        <v>456</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
@@ -21832,8 +21845,11 @@
         <f>IF(D6="","",IF(OR(H6="S",M6="S",R6="S",W6="S",AB6="S",AG6="S",AL6="S"),"S","N"))</f>
         <v>N</v>
       </c>
+      <c r="AS6" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -21896,8 +21912,11 @@
         <f t="shared" ref="AR7:AR70" si="1">IF(D7="","",IF(OR(H7="S",M7="S",R7="S",W7="S",AB7="S",AG7="S",AL7="S"),"S","N"))</f>
         <v>N</v>
       </c>
+      <c r="AS7" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
@@ -21960,8 +21979,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
+      <c r="AS8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
@@ -22038,8 +22060,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
+      <c r="AS9" t="s">
+        <v>458</v>
+      </c>
     </row>
-    <row r="10" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
         <v>22</v>
@@ -22100,8 +22125,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
+      <c r="AS10" t="s">
+        <v>457</v>
+      </c>
     </row>
-    <row r="11" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
@@ -22176,8 +22204,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
+      <c r="AS11" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="12" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -22252,8 +22283,11 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
+      <c r="AS12" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="13" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
@@ -22329,7 +22363,7 @@
         <v>N</v>
       </c>
     </row>
-    <row r="14" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>22</v>
@@ -22405,7 +22439,7 @@
         <v>N</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:45" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>22</v>
@@ -22481,7 +22515,7 @@
         <v>N</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:45" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9" t="s">
         <v>22</v>
@@ -40025,15 +40059,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="c3e1b4bb-9124-477c-aa49-683b9a26b58f">
@@ -40045,6 +40070,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40249,19 +40283,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890994BF-65F0-45C5-A04B-1A065C31A5EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2FEBBB-B4B0-4147-BA7E-181AD49E4B6A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c3e1b4bb-9124-477c-aa49-683b9a26b58f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2FEBBB-B4B0-4147-BA7E-181AD49E4B6A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890994BF-65F0-45C5-A04B-1A065C31A5EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c3e1b4bb-9124-477c-aa49-683b9a26b58f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>